<commit_message>
updated with correct values
</commit_message>
<xml_diff>
--- a/Results_3_3.xlsx
+++ b/Results_3_3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alec\Desktop\Uni\SML\exercise 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alec\Documents\GitHub\SML\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,6 +21,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>F1 Score (what we actually need) 1 person</t>
+  </si>
+  <si>
+    <t>Generic Accuracy - BAD - 2 person</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -96,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -106,6 +117,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1059,6 +1073,982 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$22:$P$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>98.477159999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8147-4D1A-B5EE-414D4549204C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$23:$P$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>97.698210000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.172240000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8147-4D1A-B5EE-414D4549204C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$24:$P$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>97.959180000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.959180000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.828860000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8147-4D1A-B5EE-414D4549204C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$25:$P$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>97.828860000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.698210000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98.218829999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.103899999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8147-4D1A-B5EE-414D4549204C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$26:$P$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>97.959180000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98.089169999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.959180000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.435900000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>94.736840000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8147-4D1A-B5EE-414D4549204C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>6</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$27:$P$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>97.828860000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.698210000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.567220000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.567220000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96.640829999999994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93.617019999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-8147-4D1A-B5EE-414D4549204C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>7</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$28:$P$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>97.959180000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.828860000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.698210000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.698210000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.039900000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95.150720000000007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>92.18329</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-8147-4D1A-B5EE-414D4549204C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>8</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$P$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>97.567220000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.698210000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.435900000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.698210000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.172240000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95.424840000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>94.319680000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90.109889999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-8147-4D1A-B5EE-414D4549204C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>9</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$30:$P$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>97.304239999999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.567220000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.435900000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.435900000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.304239999999993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.373059999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>95.150720000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>93.333330000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>88.734350000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-8147-4D1A-B5EE-414D4549204C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>10</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$31:$P$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>97.304239999999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.304239999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.435900000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.567220000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.172240000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.640829999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>96.238650000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>94.319680000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>91.008170000000007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>87.482420000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-8147-4D1A-B5EE-414D4549204C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:v>11</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$32:$P$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>97.435900000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.435900000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.435900000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.435900000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.435900000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97.039900000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>96.373059999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95.287959999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>92.328400000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>89.958730000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.877319999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-8147-4D1A-B5EE-414D4549204C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:v>12</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$33:$P$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>97.304239999999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.172240000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.039900000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.172240000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.172240000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97.039900000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>96.50712</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95.833330000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>93.333330000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91.304349999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>89.043000000000006</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>84.559880000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-8147-4D1A-B5EE-414D4549204C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:v>13</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$34:$P$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>96.907219999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96.907219999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.039900000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.774190000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96.907219999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.907219999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>96.640829999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>96.103899999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>93.899199999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>92.473119999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90.560879999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>88.111890000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>82.005899999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-8147-4D1A-B5EE-414D4549204C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="402934192"/>
+        <c:axId val="402929272"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="402934192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="402929272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="402929272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="80"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="402934192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1099,7 +2089,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1648,6 +3194,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6976F46-74E9-407F-9FC8-AF2488B4FE5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1953,14 +3535,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:P17"/>
+  <dimension ref="C4:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
     <row r="5" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="1">
         <v>1</v>
@@ -2377,7 +3967,435 @@
         <v>57.625</v>
       </c>
     </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>98.477159999999998</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3">
+        <v>97.698210000000003</v>
+      </c>
+      <c r="E23" s="3">
+        <v>97.172240000000002</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+    </row>
+    <row r="24" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="1">
+        <v>3</v>
+      </c>
+      <c r="D24" s="2">
+        <v>97.959180000000003</v>
+      </c>
+      <c r="E24" s="2">
+        <v>97.959180000000003</v>
+      </c>
+      <c r="F24" s="2">
+        <v>97.828860000000006</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="1">
+        <v>4</v>
+      </c>
+      <c r="D25" s="3">
+        <v>97.828860000000006</v>
+      </c>
+      <c r="E25" s="3">
+        <v>97.698210000000003</v>
+      </c>
+      <c r="F25" s="3">
+        <v>98.218829999999997</v>
+      </c>
+      <c r="G25" s="3">
+        <v>96.103899999999996</v>
+      </c>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+    </row>
+    <row r="26" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="1">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2">
+        <v>97.959180000000003</v>
+      </c>
+      <c r="E26" s="2">
+        <v>98.089169999999996</v>
+      </c>
+      <c r="F26" s="2">
+        <v>97.959180000000003</v>
+      </c>
+      <c r="G26" s="2">
+        <v>97.435900000000004</v>
+      </c>
+      <c r="H26" s="2">
+        <v>94.736840000000001</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="1">
+        <v>6</v>
+      </c>
+      <c r="D27" s="3">
+        <v>97.828860000000006</v>
+      </c>
+      <c r="E27" s="3">
+        <v>97.698210000000003</v>
+      </c>
+      <c r="F27" s="3">
+        <v>97.567220000000006</v>
+      </c>
+      <c r="G27" s="3">
+        <v>97.567220000000006</v>
+      </c>
+      <c r="H27" s="3">
+        <v>96.640829999999994</v>
+      </c>
+      <c r="I27" s="3">
+        <v>93.617019999999997</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="1">
+        <v>7</v>
+      </c>
+      <c r="D28" s="2">
+        <v>97.959180000000003</v>
+      </c>
+      <c r="E28" s="2">
+        <v>97.828860000000006</v>
+      </c>
+      <c r="F28" s="2">
+        <v>97.698210000000003</v>
+      </c>
+      <c r="G28" s="2">
+        <v>97.698210000000003</v>
+      </c>
+      <c r="H28" s="2">
+        <v>97.039900000000003</v>
+      </c>
+      <c r="I28" s="2">
+        <v>95.150720000000007</v>
+      </c>
+      <c r="J28" s="2">
+        <v>92.18329</v>
+      </c>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+    </row>
+    <row r="29" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="1">
+        <v>8</v>
+      </c>
+      <c r="D29" s="3">
+        <v>97.567220000000006</v>
+      </c>
+      <c r="E29" s="3">
+        <v>97.698210000000003</v>
+      </c>
+      <c r="F29" s="3">
+        <v>97.435900000000004</v>
+      </c>
+      <c r="G29" s="3">
+        <v>97.698210000000003</v>
+      </c>
+      <c r="H29" s="3">
+        <v>97.172240000000002</v>
+      </c>
+      <c r="I29" s="3">
+        <v>95.424840000000003</v>
+      </c>
+      <c r="J29" s="3">
+        <v>94.319680000000005</v>
+      </c>
+      <c r="K29" s="3">
+        <v>90.109889999999993</v>
+      </c>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+    </row>
+    <row r="30" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="1">
+        <v>9</v>
+      </c>
+      <c r="D30" s="2">
+        <v>97.304239999999993</v>
+      </c>
+      <c r="E30" s="2">
+        <v>97.567220000000006</v>
+      </c>
+      <c r="F30" s="2">
+        <v>97.435900000000004</v>
+      </c>
+      <c r="G30" s="2">
+        <v>97.435900000000004</v>
+      </c>
+      <c r="H30" s="2">
+        <v>97.304239999999993</v>
+      </c>
+      <c r="I30" s="2">
+        <v>96.373059999999995</v>
+      </c>
+      <c r="J30" s="2">
+        <v>95.150720000000007</v>
+      </c>
+      <c r="K30" s="2">
+        <v>93.333330000000004</v>
+      </c>
+      <c r="L30" s="2">
+        <v>88.734350000000006</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+    </row>
+    <row r="31" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="1">
+        <v>10</v>
+      </c>
+      <c r="D31" s="3">
+        <v>97.304239999999993</v>
+      </c>
+      <c r="E31" s="3">
+        <v>97.304239999999993</v>
+      </c>
+      <c r="F31" s="3">
+        <v>97.435900000000004</v>
+      </c>
+      <c r="G31" s="3">
+        <v>97.567220000000006</v>
+      </c>
+      <c r="H31" s="3">
+        <v>97.172240000000002</v>
+      </c>
+      <c r="I31" s="3">
+        <v>96.640829999999994</v>
+      </c>
+      <c r="J31" s="3">
+        <v>96.238650000000007</v>
+      </c>
+      <c r="K31" s="3">
+        <v>94.319680000000005</v>
+      </c>
+      <c r="L31" s="3">
+        <v>91.008170000000007</v>
+      </c>
+      <c r="M31" s="3">
+        <v>87.482420000000005</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+    </row>
+    <row r="32" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="1">
+        <v>11</v>
+      </c>
+      <c r="D32" s="2">
+        <v>97.435900000000004</v>
+      </c>
+      <c r="E32" s="2">
+        <v>97.435900000000004</v>
+      </c>
+      <c r="F32" s="2">
+        <v>97.435900000000004</v>
+      </c>
+      <c r="G32" s="2">
+        <v>97.435900000000004</v>
+      </c>
+      <c r="H32" s="2">
+        <v>97.435900000000004</v>
+      </c>
+      <c r="I32" s="2">
+        <v>97.039900000000003</v>
+      </c>
+      <c r="J32" s="2">
+        <v>96.373059999999995</v>
+      </c>
+      <c r="K32" s="2">
+        <v>95.287959999999998</v>
+      </c>
+      <c r="L32" s="2">
+        <v>92.328400000000002</v>
+      </c>
+      <c r="M32" s="2">
+        <v>89.958730000000003</v>
+      </c>
+      <c r="N32" s="2">
+        <v>85.877319999999997</v>
+      </c>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+    </row>
+    <row r="33" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="1">
+        <v>12</v>
+      </c>
+      <c r="D33" s="3">
+        <v>97.304239999999993</v>
+      </c>
+      <c r="E33" s="3">
+        <v>97.172240000000002</v>
+      </c>
+      <c r="F33" s="3">
+        <v>97.039900000000003</v>
+      </c>
+      <c r="G33" s="3">
+        <v>97.172240000000002</v>
+      </c>
+      <c r="H33" s="3">
+        <v>97.172240000000002</v>
+      </c>
+      <c r="I33" s="3">
+        <v>97.039900000000003</v>
+      </c>
+      <c r="J33" s="3">
+        <v>96.50712</v>
+      </c>
+      <c r="K33" s="3">
+        <v>95.833330000000004</v>
+      </c>
+      <c r="L33" s="3">
+        <v>93.333330000000004</v>
+      </c>
+      <c r="M33" s="3">
+        <v>91.304349999999999</v>
+      </c>
+      <c r="N33" s="3">
+        <v>89.043000000000006</v>
+      </c>
+      <c r="O33" s="3">
+        <v>84.559880000000007</v>
+      </c>
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="1">
+        <v>13</v>
+      </c>
+      <c r="D34" s="2">
+        <v>96.907219999999995</v>
+      </c>
+      <c r="E34" s="2">
+        <v>96.907219999999995</v>
+      </c>
+      <c r="F34" s="2">
+        <v>97.039900000000003</v>
+      </c>
+      <c r="G34" s="2">
+        <v>96.774190000000004</v>
+      </c>
+      <c r="H34" s="2">
+        <v>96.907219999999995</v>
+      </c>
+      <c r="I34" s="2">
+        <v>96.907219999999995</v>
+      </c>
+      <c r="J34" s="2">
+        <v>96.640829999999994</v>
+      </c>
+      <c r="K34" s="2">
+        <v>96.103899999999996</v>
+      </c>
+      <c r="L34" s="2">
+        <v>93.899199999999993</v>
+      </c>
+      <c r="M34" s="2">
+        <v>92.473119999999994</v>
+      </c>
+      <c r="N34" s="2">
+        <v>90.560879999999997</v>
+      </c>
+      <c r="O34" s="2">
+        <v>88.111890000000002</v>
+      </c>
+      <c r="P34" s="2">
+        <v>82.005899999999997</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C21:F21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>